<commit_message>
Edit and export Mario Gantt
</commit_message>
<xml_diff>
--- a/pp/gantt/MarioTasksAllocation.xlsx
+++ b/pp/gantt/MarioTasksAllocation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Task #</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Outline Level</t>
   </si>
   <si>
-    <t>Davide</t>
-  </si>
-  <si>
     <t>Mario</t>
   </si>
   <si>
@@ -126,6 +123,21 @@
   </si>
   <si>
     <t>Revision and requirement traceability</t>
+  </si>
+  <si>
+    <t>Document revision</t>
+  </si>
+  <si>
+    <t>Integration test strategy</t>
+  </si>
+  <si>
+    <t>Definition of precedences</t>
+  </si>
+  <si>
+    <t>Sequence of components integration</t>
+  </si>
+  <si>
+    <t>Program Drivers</t>
   </si>
 </sst>
 </file>
@@ -488,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +544,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D25" si="0">CONCATENATE(NETWORKDAYS(E2,F2),"g")</f>
+        <f t="shared" ref="D2:D31" si="0">CONCATENATE(NETWORKDAYS(E2,F2),"g")</f>
         <v>40g</v>
       </c>
       <c r="E2" s="2">
@@ -553,10 +565,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -577,10 +589,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -601,10 +613,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -625,10 +637,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -649,10 +661,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -673,10 +685,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -697,10 +709,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -721,7 +733,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -742,10 +754,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -766,20 +778,20 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="E12" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="F12" s="2">
-        <v>42687.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -790,20 +802,20 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>3g</v>
       </c>
       <c r="E13" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="F13" s="2">
-        <v>42687.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -814,23 +826,23 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>4g</v>
       </c>
       <c r="E14" s="2">
-        <v>42677.333333333336</v>
+        <v>42682.333333333336</v>
       </c>
       <c r="F14" s="2">
         <v>42685.666666666664</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -838,23 +850,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>3g</v>
       </c>
       <c r="E15" s="2">
-        <v>42688.333333333336</v>
+        <v>42677.333333333336</v>
       </c>
       <c r="F15" s="2">
-        <v>42690.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -862,10 +871,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -878,18 +887,18 @@
         <v>42690.666666666664</v>
       </c>
       <c r="G16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -905,15 +914,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -929,170 +938,321 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>2g</v>
+        <v>3g</v>
       </c>
       <c r="E19" s="2">
-        <v>42691.333333333336</v>
+        <v>42688.333333333336</v>
       </c>
       <c r="F19" s="2">
-        <v>42692.666666666664</v>
+        <v>42690.666666666664</v>
       </c>
       <c r="G19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>1g</v>
       </c>
       <c r="E20" s="2">
-        <v>42695.333333333336</v>
+        <v>42691.333333333336</v>
       </c>
       <c r="F20" s="2">
-        <v>42697.666666666664</v>
+        <v>42691.666666666664</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>2g</v>
       </c>
       <c r="E21" s="2">
-        <v>42698.333333333336</v>
+        <v>42692.333333333336</v>
       </c>
       <c r="F21" s="2">
-        <v>42702.666666666664</v>
+        <v>42695.666666666664</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>2g</v>
       </c>
       <c r="E22" s="2">
-        <v>42703.333333333336</v>
+        <v>42696.333333333336</v>
       </c>
       <c r="F22" s="2">
-        <v>42704.666666666664</v>
+        <v>42697.666666666664</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>1g</v>
+        <v>2g</v>
       </c>
       <c r="E23" s="2">
-        <v>42705.333333333336</v>
+        <v>42698.333333333336</v>
       </c>
       <c r="F23" s="2">
-        <v>42705.666666666664</v>
+        <v>42699.666666666664</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
         <v>31</v>
       </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>1g</v>
       </c>
       <c r="E24" s="2">
-        <v>42711.333333333336</v>
+        <v>42702.333333333336</v>
       </c>
       <c r="F24" s="2">
-        <v>42711.666666666664</v>
+        <v>42702.666666666664</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E25" s="2">
+        <v>42705.333333333336</v>
+      </c>
+      <c r="F25" s="2">
+        <v>42705.666666666664</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E26" s="2">
+        <v>42706.333333333336</v>
+      </c>
+      <c r="F26" s="2">
+        <v>42706.666666666664</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E27" s="2">
+        <v>42716.333333333336</v>
+      </c>
+      <c r="F27" s="2">
+        <v>42716.666666666664</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E28" s="2">
+        <v>42716.333333333336</v>
+      </c>
+      <c r="F28" s="2">
+        <v>42716.666666666664</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>2g</v>
+      </c>
+      <c r="E29" s="2">
+        <v>42717.333333333336</v>
+      </c>
+      <c r="F29" s="2">
+        <v>42718.666666666664</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E30" s="2">
+        <v>42719.333333333336</v>
+      </c>
+      <c r="F30" s="2">
+        <v>42719.666666666664</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>1g</v>
-      </c>
-      <c r="E25" s="2">
-        <v>42713.333333333336</v>
-      </c>
-      <c r="F25" s="2">
-        <v>42713.666666666664</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>2g</v>
+      </c>
+      <c r="E31" s="2">
+        <v>42720.333333333336</v>
+      </c>
+      <c r="F31" s="2">
+        <v>42723.666666666664</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed and re exported Mario Gantt
</commit_message>
<xml_diff>
--- a/pp/gantt/MarioTasksAllocation.xlsx
+++ b/pp/gantt/MarioTasksAllocation.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A31"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,47 +823,47 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>4g</v>
+        <v>3g</v>
       </c>
       <c r="E14" s="2">
-        <v>42682.333333333336</v>
+        <v>42677.333333333336</v>
       </c>
       <c r="F14" s="2">
-        <v>42685.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>3g</v>
+        <f>CONCATENATE(NETWORKDAYS(E15,F15),"g")</f>
+        <v>4g</v>
       </c>
       <c r="E15" s="2">
-        <v>42677.333333333336</v>
+        <v>42682.333333333336</v>
       </c>
       <c r="F15" s="2">
-        <v>42681.666666666664</v>
+        <v>42685.666666666664</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
calculate the actual wokdays in excel
</commit_message>
<xml_diff>
--- a/pp/gantt/MarioTasksAllocation.xlsx
+++ b/pp/gantt/MarioTasksAllocation.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -583,8 +583,11 @@
       <c r="G3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -608,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -632,7 +635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -655,8 +658,11 @@
       <c r="G6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -680,7 +686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -704,7 +710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -728,7 +734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -748,8 +754,11 @@
       <c r="G10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -772,8 +781,11 @@
       <c r="G11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -796,8 +808,11 @@
       <c r="G12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -821,7 +836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -842,7 +857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -865,8 +880,11 @@
       <c r="G15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -887,6 +905,9 @@
         <v>42690.666666666664</v>
       </c>
       <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
         <v>2</v>
       </c>
     </row>
@@ -985,6 +1006,9 @@
       <c r="G20">
         <v>2</v>
       </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1009,6 +1033,9 @@
       <c r="G21">
         <v>2</v>
       </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1033,6 +1060,9 @@
       <c r="G22">
         <v>2</v>
       </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1054,6 +1084,9 @@
       <c r="G23">
         <v>2</v>
       </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1078,6 +1111,9 @@
       <c r="G24">
         <v>2</v>
       </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1102,6 +1138,9 @@
       <c r="G25">
         <v>2</v>
       </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1126,6 +1165,9 @@
       <c r="G26">
         <v>2</v>
       </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1150,6 +1192,9 @@
       <c r="G27">
         <v>2</v>
       </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
@@ -1175,6 +1220,9 @@
       </c>
       <c r="G28">
         <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>

</xml_diff>